<commit_message>
Split Code into functions, improve save (Full Operation)
</commit_message>
<xml_diff>
--- a/Project_Insight/bin/Debug/Programs.xlsx
+++ b/Project_Insight/bin/Debug/Programs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13545" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VyM" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="45">
   <si>
     <t>Presidente:</t>
   </si>
@@ -279,16 +279,10 @@
     <t>3 DE NOVIEMBRE</t>
   </si>
   <si>
-    <t xml:space="preserve">Sabado </t>
+    <t xml:space="preserve"> (10 mins.)</t>
   </si>
   <si>
-    <t xml:space="preserve">Lunes </t>
-  </si>
-  <si>
-    <t>Aseo Grupo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (10 mins.)</t>
+    <t>Aseo:</t>
   </si>
 </sst>
 </file>
@@ -947,23 +941,65 @@
     <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -971,44 +1007,32 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1016,38 +1040,14 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1066,12 +1066,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1362,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -1396,22 +1390,22 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
       <c r="F3" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1459,13 +1453,13 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
         <v>9</v>
@@ -1478,12 +1472,12 @@
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
+      <c r="C9" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1532,13 +1526,13 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
         <v>9</v>
@@ -1551,11 +1545,11 @@
       <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
       <c r="F14" s="51"/>
       <c r="G14" s="13"/>
     </row>
@@ -1566,11 +1560,11 @@
       <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="60" t="s">
+      <c r="C15" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
     </row>
@@ -1581,11 +1575,11 @@
       <c r="B16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
     </row>
@@ -1605,13 +1599,13 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="67" t="s">
+      <c r="A18" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
@@ -1637,34 +1631,34 @@
       <c r="B20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="70">
         <v>0.33819444444444446</v>
       </c>
-      <c r="B22" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="60" t="s">
+      <c r="B22" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
       <c r="F22" s="3" t="s">
         <v>25</v>
       </c>
@@ -1672,10 +1666,10 @@
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="70"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
       <c r="F23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1688,12 +1682,12 @@
       <c r="B24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1734,22 +1728,22 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
+      <c r="A28" s="63"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
       <c r="F28" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G28" s="34"/>
     </row>
     <row r="29" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
+      <c r="A29" s="65"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
       <c r="F29" s="3" t="s">
         <v>1</v>
       </c>
@@ -1797,13 +1791,13 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4" t="s">
         <v>9</v>
@@ -1816,12 +1810,12 @@
       <c r="B34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
+      <c r="C34" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
       <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1870,13 +1864,13 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="64"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4" t="s">
         <v>9</v>
@@ -1889,11 +1883,11 @@
       <c r="B39" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="60" t="s">
+      <c r="C39" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
       <c r="F39" s="51"/>
       <c r="G39" s="13"/>
     </row>
@@ -1904,11 +1898,11 @@
       <c r="B40" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="60" t="s">
+      <c r="C40" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
     </row>
@@ -1919,11 +1913,11 @@
       <c r="B41" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="60" t="s">
+      <c r="C41" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
     </row>
@@ -1943,13 +1937,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="67" t="s">
+      <c r="A43" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B43" s="68"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
@@ -1975,35 +1969,35 @@
       <c r="B45" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
       <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="54"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
       <c r="G46" s="52"/>
     </row>
     <row r="47" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="70">
         <v>0.33819444444444446</v>
       </c>
-      <c r="B47" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="60" t="s">
+      <c r="B47" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
       <c r="F47" s="3" t="s">
         <v>25</v>
       </c>
@@ -2011,10 +2005,10 @@
     </row>
     <row r="48" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="70"/>
-      <c r="B48" s="71"/>
-      <c r="C48" s="60"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="60"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
       <c r="F48" s="3" t="s">
         <v>27</v>
       </c>
@@ -2027,12 +2021,12 @@
       <c r="B49" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="60" t="s">
+      <c r="C49" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="60"/>
-      <c r="E49" s="60"/>
-      <c r="F49" s="60"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
       <c r="G49" s="14"/>
     </row>
     <row r="50" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2071,14 +2065,14 @@
       <c r="G52" s="9"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="61" t="s">
+      <c r="A53" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="61"/>
-      <c r="C53" s="61"/>
-      <c r="D53" s="61"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="62"/>
+      <c r="B53" s="75"/>
+      <c r="C53" s="75"/>
+      <c r="D53" s="75"/>
+      <c r="E53" s="75"/>
+      <c r="F53" s="76"/>
       <c r="G53" s="10" t="s">
         <v>14</v>
       </c>
@@ -2102,22 +2096,22 @@
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="55"/>
-      <c r="B56" s="55"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="55"/>
-      <c r="E56" s="55"/>
+      <c r="A56" s="63"/>
+      <c r="B56" s="63"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="63"/>
+      <c r="E56" s="63"/>
       <c r="F56" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G56" s="34"/>
     </row>
     <row r="57" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="56"/>
-      <c r="B57" s="56"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="56"/>
-      <c r="E57" s="56"/>
+      <c r="A57" s="65"/>
+      <c r="B57" s="65"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="65"/>
+      <c r="E57" s="65"/>
       <c r="F57" s="3" t="s">
         <v>1</v>
       </c>
@@ -2165,13 +2159,13 @@
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="65" t="s">
+      <c r="A61" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="65"/>
-      <c r="C61" s="66"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="66"/>
+      <c r="B61" s="67"/>
+      <c r="C61" s="68"/>
+      <c r="D61" s="68"/>
+      <c r="E61" s="68"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4" t="s">
         <v>9</v>
@@ -2184,12 +2178,12 @@
       <c r="B62" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" s="60"/>
-      <c r="E62" s="60"/>
-      <c r="F62" s="60"/>
+      <c r="C62" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D62" s="56"/>
+      <c r="E62" s="56"/>
+      <c r="F62" s="56"/>
       <c r="G62" s="12"/>
     </row>
     <row r="63" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2238,13 +2232,13 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="63" t="s">
+      <c r="A66" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="64"/>
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
-      <c r="E66" s="64"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="61"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="61"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4" t="s">
         <v>9</v>
@@ -2257,11 +2251,11 @@
       <c r="B67" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="60" t="s">
+      <c r="C67" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D67" s="60"/>
-      <c r="E67" s="60"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="56"/>
       <c r="F67" s="51"/>
       <c r="G67" s="13"/>
     </row>
@@ -2272,11 +2266,11 @@
       <c r="B68" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="60" t="s">
+      <c r="C68" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="60"/>
-      <c r="E68" s="60"/>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
     </row>
@@ -2287,11 +2281,11 @@
       <c r="B69" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="60" t="s">
+      <c r="C69" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="D69" s="60"/>
-      <c r="E69" s="60"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="56"/>
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
     </row>
@@ -2311,13 +2305,13 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="67" t="s">
+      <c r="A71" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B71" s="68"/>
-      <c r="C71" s="68"/>
-      <c r="D71" s="68"/>
-      <c r="E71" s="68"/>
+      <c r="B71" s="58"/>
+      <c r="C71" s="58"/>
+      <c r="D71" s="58"/>
+      <c r="E71" s="58"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
     </row>
@@ -2343,35 +2337,35 @@
       <c r="B73" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C73" s="60" t="s">
+      <c r="C73" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="60"/>
-      <c r="E73" s="60"/>
-      <c r="F73" s="60"/>
+      <c r="D73" s="56"/>
+      <c r="E73" s="56"/>
+      <c r="F73" s="56"/>
       <c r="G73" s="12"/>
     </row>
     <row r="74" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="54"/>
-      <c r="C74" s="60"/>
-      <c r="D74" s="60"/>
-      <c r="E74" s="60"/>
-      <c r="F74" s="60"/>
+      <c r="C74" s="56"/>
+      <c r="D74" s="56"/>
+      <c r="E74" s="56"/>
+      <c r="F74" s="56"/>
       <c r="G74" s="52"/>
     </row>
     <row r="75" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="70">
         <v>0.33819444444444446</v>
       </c>
-      <c r="B75" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75" s="60" t="s">
+      <c r="B75" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D75" s="60"/>
-      <c r="E75" s="60"/>
+      <c r="D75" s="56"/>
+      <c r="E75" s="56"/>
       <c r="F75" s="3" t="s">
         <v>25</v>
       </c>
@@ -2379,10 +2373,10 @@
     </row>
     <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="70"/>
-      <c r="B76" s="71"/>
-      <c r="C76" s="60"/>
-      <c r="D76" s="60"/>
-      <c r="E76" s="60"/>
+      <c r="B76" s="69"/>
+      <c r="C76" s="56"/>
+      <c r="D76" s="56"/>
+      <c r="E76" s="56"/>
       <c r="F76" s="3" t="s">
         <v>27</v>
       </c>
@@ -2395,12 +2389,12 @@
       <c r="B77" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="60" t="s">
+      <c r="C77" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D77" s="60"/>
-      <c r="E77" s="60"/>
-      <c r="F77" s="60"/>
+      <c r="D77" s="56"/>
+      <c r="E77" s="56"/>
+      <c r="F77" s="56"/>
       <c r="G77" s="14"/>
     </row>
     <row r="78" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2439,22 +2433,22 @@
       <c r="G80" s="2"/>
     </row>
     <row r="81" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="55"/>
-      <c r="B81" s="55"/>
-      <c r="C81" s="57"/>
-      <c r="D81" s="55"/>
-      <c r="E81" s="55"/>
+      <c r="A81" s="63"/>
+      <c r="B81" s="63"/>
+      <c r="C81" s="64"/>
+      <c r="D81" s="63"/>
+      <c r="E81" s="63"/>
       <c r="F81" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G81" s="34"/>
     </row>
     <row r="82" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="56"/>
-      <c r="B82" s="56"/>
-      <c r="C82" s="58"/>
-      <c r="D82" s="56"/>
-      <c r="E82" s="56"/>
+      <c r="A82" s="65"/>
+      <c r="B82" s="65"/>
+      <c r="C82" s="66"/>
+      <c r="D82" s="65"/>
+      <c r="E82" s="65"/>
       <c r="F82" s="3" t="s">
         <v>1</v>
       </c>
@@ -2502,13 +2496,13 @@
       <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="65" t="s">
+      <c r="A86" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B86" s="65"/>
-      <c r="C86" s="66"/>
-      <c r="D86" s="66"/>
-      <c r="E86" s="66"/>
+      <c r="B86" s="67"/>
+      <c r="C86" s="68"/>
+      <c r="D86" s="68"/>
+      <c r="E86" s="68"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4" t="s">
         <v>9</v>
@@ -2521,12 +2515,12 @@
       <c r="B87" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="D87" s="60"/>
-      <c r="E87" s="60"/>
-      <c r="F87" s="60"/>
+      <c r="C87" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D87" s="56"/>
+      <c r="E87" s="56"/>
+      <c r="F87" s="56"/>
       <c r="G87" s="12"/>
     </row>
     <row r="88" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2575,13 +2569,13 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="63" t="s">
+      <c r="A91" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="64"/>
-      <c r="C91" s="64"/>
-      <c r="D91" s="64"/>
-      <c r="E91" s="64"/>
+      <c r="B91" s="61"/>
+      <c r="C91" s="61"/>
+      <c r="D91" s="61"/>
+      <c r="E91" s="61"/>
       <c r="F91" s="4"/>
       <c r="G91" s="4" t="s">
         <v>9</v>
@@ -2594,11 +2588,11 @@
       <c r="B92" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C92" s="60" t="s">
+      <c r="C92" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D92" s="60"/>
-      <c r="E92" s="60"/>
+      <c r="D92" s="56"/>
+      <c r="E92" s="56"/>
       <c r="F92" s="51"/>
       <c r="G92" s="13"/>
     </row>
@@ -2609,11 +2603,11 @@
       <c r="B93" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C93" s="60" t="s">
+      <c r="C93" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D93" s="60"/>
-      <c r="E93" s="60"/>
+      <c r="D93" s="56"/>
+      <c r="E93" s="56"/>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
     </row>
@@ -2624,11 +2618,11 @@
       <c r="B94" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C94" s="60" t="s">
+      <c r="C94" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="60"/>
-      <c r="E94" s="60"/>
+      <c r="D94" s="56"/>
+      <c r="E94" s="56"/>
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
     </row>
@@ -2648,13 +2642,13 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="67" t="s">
+      <c r="A96" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B96" s="68"/>
-      <c r="C96" s="68"/>
-      <c r="D96" s="68"/>
-      <c r="E96" s="68"/>
+      <c r="B96" s="58"/>
+      <c r="C96" s="58"/>
+      <c r="D96" s="58"/>
+      <c r="E96" s="58"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
     </row>
@@ -2680,35 +2674,35 @@
       <c r="B98" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C98" s="60" t="s">
+      <c r="C98" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="D98" s="60"/>
-      <c r="E98" s="60"/>
-      <c r="F98" s="60"/>
+      <c r="D98" s="56"/>
+      <c r="E98" s="56"/>
+      <c r="F98" s="56"/>
       <c r="G98" s="12"/>
     </row>
     <row r="99" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="B99" s="54"/>
-      <c r="C99" s="60"/>
-      <c r="D99" s="60"/>
-      <c r="E99" s="60"/>
-      <c r="F99" s="60"/>
+      <c r="C99" s="56"/>
+      <c r="D99" s="56"/>
+      <c r="E99" s="56"/>
+      <c r="F99" s="56"/>
       <c r="G99" s="52"/>
     </row>
     <row r="100" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="70">
         <v>0.33819444444444446</v>
       </c>
-      <c r="B100" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="C100" s="60" t="s">
+      <c r="B100" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D100" s="60"/>
-      <c r="E100" s="60"/>
+      <c r="D100" s="56"/>
+      <c r="E100" s="56"/>
       <c r="F100" s="3" t="s">
         <v>25</v>
       </c>
@@ -2716,10 +2710,10 @@
     </row>
     <row r="101" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="70"/>
-      <c r="B101" s="71"/>
-      <c r="C101" s="60"/>
-      <c r="D101" s="60"/>
-      <c r="E101" s="60"/>
+      <c r="B101" s="69"/>
+      <c r="C101" s="56"/>
+      <c r="D101" s="56"/>
+      <c r="E101" s="56"/>
       <c r="F101" s="3" t="s">
         <v>27</v>
       </c>
@@ -2732,12 +2726,12 @@
       <c r="B102" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C102" s="60" t="s">
+      <c r="C102" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D102" s="60"/>
-      <c r="E102" s="60"/>
-      <c r="F102" s="60"/>
+      <c r="D102" s="56"/>
+      <c r="E102" s="56"/>
+      <c r="F102" s="56"/>
       <c r="G102" s="14"/>
     </row>
     <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2776,12 +2770,12 @@
       <c r="G105" s="9"/>
     </row>
     <row r="106" spans="1:7" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="74"/>
-      <c r="B106" s="74"/>
-      <c r="C106" s="74"/>
-      <c r="D106" s="74"/>
-      <c r="E106" s="74"/>
-      <c r="F106" s="75"/>
+      <c r="A106" s="73"/>
+      <c r="B106" s="73"/>
+      <c r="C106" s="73"/>
+      <c r="D106" s="73"/>
+      <c r="E106" s="73"/>
+      <c r="F106" s="74"/>
       <c r="G106" s="10" t="s">
         <v>15</v>
       </c>
@@ -2805,22 +2799,22 @@
       <c r="G108" s="2"/>
     </row>
     <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="55"/>
-      <c r="B109" s="55"/>
-      <c r="C109" s="57"/>
-      <c r="D109" s="55"/>
-      <c r="E109" s="55"/>
+      <c r="A109" s="63"/>
+      <c r="B109" s="63"/>
+      <c r="C109" s="64"/>
+      <c r="D109" s="63"/>
+      <c r="E109" s="63"/>
       <c r="F109" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G109" s="34"/>
     </row>
     <row r="110" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="56"/>
-      <c r="B110" s="56"/>
-      <c r="C110" s="58"/>
-      <c r="D110" s="56"/>
-      <c r="E110" s="56"/>
+      <c r="A110" s="65"/>
+      <c r="B110" s="65"/>
+      <c r="C110" s="66"/>
+      <c r="D110" s="65"/>
+      <c r="E110" s="65"/>
       <c r="F110" s="3" t="s">
         <v>1</v>
       </c>
@@ -2868,13 +2862,13 @@
       <c r="G113" s="2"/>
     </row>
     <row r="114" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="65" t="s">
+      <c r="A114" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B114" s="65"/>
-      <c r="C114" s="66"/>
-      <c r="D114" s="66"/>
-      <c r="E114" s="66"/>
+      <c r="B114" s="67"/>
+      <c r="C114" s="68"/>
+      <c r="D114" s="68"/>
+      <c r="E114" s="68"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4" t="s">
         <v>9</v>
@@ -2887,12 +2881,12 @@
       <c r="B115" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C115" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="D115" s="60"/>
-      <c r="E115" s="60"/>
-      <c r="F115" s="60"/>
+      <c r="C115" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D115" s="56"/>
+      <c r="E115" s="56"/>
+      <c r="F115" s="56"/>
       <c r="G115" s="12"/>
     </row>
     <row r="116" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2941,13 +2935,13 @@
       </c>
     </row>
     <row r="119" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="63" t="s">
+      <c r="A119" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B119" s="64"/>
-      <c r="C119" s="64"/>
-      <c r="D119" s="64"/>
-      <c r="E119" s="64"/>
+      <c r="B119" s="61"/>
+      <c r="C119" s="61"/>
+      <c r="D119" s="61"/>
+      <c r="E119" s="61"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4" t="s">
         <v>9</v>
@@ -2960,11 +2954,11 @@
       <c r="B120" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C120" s="60" t="s">
+      <c r="C120" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="D120" s="60"/>
-      <c r="E120" s="60"/>
+      <c r="D120" s="56"/>
+      <c r="E120" s="56"/>
       <c r="F120" s="51"/>
       <c r="G120" s="13"/>
     </row>
@@ -2975,11 +2969,11 @@
       <c r="B121" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C121" s="60" t="s">
+      <c r="C121" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D121" s="60"/>
-      <c r="E121" s="60"/>
+      <c r="D121" s="56"/>
+      <c r="E121" s="56"/>
       <c r="F121" s="13"/>
       <c r="G121" s="13"/>
     </row>
@@ -2990,11 +2984,11 @@
       <c r="B122" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C122" s="60" t="s">
+      <c r="C122" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="D122" s="60"/>
-      <c r="E122" s="60"/>
+      <c r="D122" s="56"/>
+      <c r="E122" s="56"/>
       <c r="F122" s="13"/>
       <c r="G122" s="13"/>
     </row>
@@ -3014,13 +3008,13 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="67" t="s">
+      <c r="A124" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B124" s="68"/>
-      <c r="C124" s="68"/>
-      <c r="D124" s="68"/>
-      <c r="E124" s="68"/>
+      <c r="B124" s="58"/>
+      <c r="C124" s="58"/>
+      <c r="D124" s="58"/>
+      <c r="E124" s="58"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
     </row>
@@ -3046,35 +3040,35 @@
       <c r="B126" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C126" s="60" t="s">
+      <c r="C126" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="D126" s="60"/>
-      <c r="E126" s="60"/>
-      <c r="F126" s="60"/>
+      <c r="D126" s="56"/>
+      <c r="E126" s="56"/>
+      <c r="F126" s="56"/>
       <c r="G126" s="12"/>
     </row>
     <row r="127" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6"/>
       <c r="B127" s="54"/>
-      <c r="C127" s="60"/>
-      <c r="D127" s="60"/>
-      <c r="E127" s="60"/>
-      <c r="F127" s="60"/>
+      <c r="C127" s="56"/>
+      <c r="D127" s="56"/>
+      <c r="E127" s="56"/>
+      <c r="F127" s="56"/>
       <c r="G127" s="52"/>
     </row>
     <row r="128" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="70">
         <v>0.33819444444444446</v>
       </c>
-      <c r="B128" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="C128" s="60" t="s">
+      <c r="B128" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D128" s="60"/>
-      <c r="E128" s="60"/>
+      <c r="D128" s="56"/>
+      <c r="E128" s="56"/>
       <c r="F128" s="3" t="s">
         <v>25</v>
       </c>
@@ -3082,10 +3076,10 @@
     </row>
     <row r="129" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="70"/>
-      <c r="B129" s="71"/>
-      <c r="C129" s="60"/>
-      <c r="D129" s="60"/>
-      <c r="E129" s="60"/>
+      <c r="B129" s="69"/>
+      <c r="C129" s="56"/>
+      <c r="D129" s="56"/>
+      <c r="E129" s="56"/>
       <c r="F129" s="3" t="s">
         <v>27</v>
       </c>
@@ -3098,12 +3092,12 @@
       <c r="B130" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C130" s="60" t="s">
+      <c r="C130" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D130" s="60"/>
-      <c r="E130" s="60"/>
-      <c r="F130" s="60"/>
+      <c r="D130" s="56"/>
+      <c r="E130" s="56"/>
+      <c r="F130" s="56"/>
       <c r="G130" s="14"/>
     </row>
     <row r="131" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3349,12 +3343,12 @@
       <c r="G156" s="2"/>
     </row>
     <row r="157" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="72"/>
-      <c r="B157" s="72"/>
-      <c r="C157" s="72"/>
-      <c r="D157" s="72"/>
-      <c r="E157" s="72"/>
-      <c r="F157" s="73"/>
+      <c r="A157" s="71"/>
+      <c r="B157" s="71"/>
+      <c r="C157" s="71"/>
+      <c r="D157" s="71"/>
+      <c r="E157" s="71"/>
+      <c r="F157" s="72"/>
       <c r="G157" s="10" t="s">
         <v>16</v>
       </c>
@@ -3433,56 +3427,20 @@
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="C126:F126"/>
-    <mergeCell ref="A124:E124"/>
-    <mergeCell ref="C125:E125"/>
-    <mergeCell ref="C116:F116"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="A119:E119"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="C115:F115"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="C99:F99"/>
-    <mergeCell ref="C77:F77"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C87:F87"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C111:E111"/>
-    <mergeCell ref="A81:C82"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C88:F88"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A86:E86"/>
-    <mergeCell ref="C75:E76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A71:E71"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C22:E23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="C63:F63"/>
+    <mergeCell ref="D109:E110"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="A3:C4"/>
+    <mergeCell ref="A28:C29"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="A56:C57"/>
+    <mergeCell ref="D56:E57"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="A66:E66"/>
     <mergeCell ref="A157:F157"/>
     <mergeCell ref="C94:E94"/>
     <mergeCell ref="A106:F106"/>
@@ -3499,7 +3457,11 @@
     <mergeCell ref="C127:F127"/>
     <mergeCell ref="C112:G112"/>
     <mergeCell ref="A114:E114"/>
-    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C22:E23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="C63:F63"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="A43:E43"/>
@@ -3511,26 +3473,58 @@
     <mergeCell ref="A61:E61"/>
     <mergeCell ref="C62:F62"/>
     <mergeCell ref="A47:A48"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A86:E86"/>
+    <mergeCell ref="C75:E76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A71:E71"/>
+    <mergeCell ref="C67:E67"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="C47:E48"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="C41:E41"/>
     <mergeCell ref="D81:E82"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C115:F115"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="C99:F99"/>
+    <mergeCell ref="C77:F77"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C87:F87"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C111:E111"/>
+    <mergeCell ref="A81:C82"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C88:F88"/>
     <mergeCell ref="A109:C110"/>
-    <mergeCell ref="D109:E110"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="A3:C4"/>
-    <mergeCell ref="A28:C29"/>
-    <mergeCell ref="D28:E29"/>
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="D56:E57"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="C126:F126"/>
+    <mergeCell ref="A124:E124"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="A119:E119"/>
+    <mergeCell ref="C120:E120"/>
   </mergeCells>
   <pageMargins left="0.79" right="0.75" top="0.58333333333333337" bottom="0.4375" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3546,8 +3540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61:G61"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3593,27 +3587,27 @@
       <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81" t="s">
+      <c r="B4" s="84"/>
+      <c r="C4" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="81"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="24"/>
       <c r="H4" s="44"/>
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
       <c r="F5" s="39"/>
       <c r="G5" s="3" t="s">
         <v>0</v>
@@ -3628,10 +3622,10 @@
       <c r="C6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
       <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3643,9 +3637,9 @@
         <v>23</v>
       </c>
       <c r="D7" s="59"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
       <c r="H7" s="43"/>
     </row>
     <row r="8" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3659,13 +3653,13 @@
       <c r="H8" s="43"/>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
       <c r="F9" s="38"/>
       <c r="G9" s="3" t="s">
         <v>25</v>
@@ -3680,9 +3674,9 @@
       <c r="C10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
       <c r="G10" s="3" t="s">
         <v>27</v>
       </c>
@@ -3692,9 +3686,9 @@
       <c r="A11" s="6"/>
       <c r="B11" s="18"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
       <c r="G11" s="3" t="s">
         <v>34</v>
       </c>
@@ -3711,64 +3705,64 @@
       <c r="H12" s="46"/>
     </row>
     <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
       <c r="G13" s="21"/>
       <c r="H13" s="46"/>
     </row>
     <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
       <c r="H14" s="41"/>
     </row>
     <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
-      <c r="C15" s="80" t="s">
+      <c r="C15" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80" t="s">
+      <c r="D15" s="82"/>
+      <c r="E15" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
       <c r="H15" s="41"/>
     </row>
     <row r="16" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="81"/>
-      <c r="C17" s="81" t="s">
+      <c r="B17" s="84"/>
+      <c r="C17" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="81"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="24"/>
       <c r="H17" s="44"/>
     </row>
     <row r="18" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="85" t="s">
+      <c r="A18" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="85"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
       <c r="F18" s="39"/>
       <c r="G18" s="3" t="s">
         <v>0</v>
@@ -3783,10 +3777,10 @@
       <c r="C19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="83"/>
       <c r="H19" s="40"/>
     </row>
     <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3798,9 +3792,9 @@
         <v>23</v>
       </c>
       <c r="D20" s="59"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="83"/>
       <c r="H20" s="43"/>
     </row>
     <row r="21" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3814,13 +3808,13 @@
       <c r="H21" s="43"/>
     </row>
     <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="84" t="s">
+      <c r="A22" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="84"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
       <c r="F22" s="38"/>
       <c r="G22" s="3" t="s">
         <v>25</v>
@@ -3835,9 +3829,9 @@
       <c r="C23" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="81"/>
       <c r="G23" s="3" t="s">
         <v>27</v>
       </c>
@@ -3847,9 +3841,9 @@
       <c r="A24" s="6"/>
       <c r="B24" s="18"/>
       <c r="C24" s="17"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
       <c r="G24" s="3" t="s">
         <v>34</v>
       </c>
@@ -3866,64 +3860,64 @@
       <c r="H25" s="46"/>
     </row>
     <row r="26" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="82"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
       <c r="G26" s="21"/>
       <c r="H26" s="46"/>
     </row>
     <row r="27" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="80"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
       <c r="H27" s="41"/>
     </row>
     <row r="28" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80" t="s">
+      <c r="D28" s="82"/>
+      <c r="E28" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="80"/>
-      <c r="G28" s="80"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
       <c r="H28" s="41"/>
     </row>
     <row r="29" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="81" t="s">
+      <c r="A30" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="81"/>
-      <c r="C30" s="81" t="s">
+      <c r="B30" s="84"/>
+      <c r="C30" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="81"/>
+      <c r="D30" s="84"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="24"/>
       <c r="H30" s="44"/>
     </row>
     <row r="31" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="85" t="s">
+      <c r="A31" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="85"/>
-      <c r="C31" s="85"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
       <c r="F31" s="39"/>
       <c r="G31" s="3" t="s">
         <v>0</v>
@@ -3938,10 +3932,10 @@
       <c r="C32" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="78"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="83"/>
       <c r="H32" s="40"/>
     </row>
     <row r="33" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3953,9 +3947,9 @@
         <v>23</v>
       </c>
       <c r="D33" s="59"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
+      <c r="E33" s="83"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
       <c r="H33" s="43"/>
     </row>
     <row r="34" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3969,13 +3963,13 @@
       <c r="H34" s="43"/>
     </row>
     <row r="35" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="84" t="s">
+      <c r="A35" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="84"/>
-      <c r="C35" s="84"/>
-      <c r="D35" s="84"/>
-      <c r="E35" s="84"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
       <c r="F35" s="38"/>
       <c r="G35" s="3" t="s">
         <v>25</v>
@@ -3990,9 +3984,9 @@
       <c r="C36" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="81"/>
       <c r="G36" s="3" t="s">
         <v>27</v>
       </c>
@@ -4002,9 +3996,9 @@
       <c r="A37" s="6"/>
       <c r="B37" s="18"/>
       <c r="C37" s="17"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="81"/>
       <c r="G37" s="3" t="s">
         <v>34</v>
       </c>
@@ -4021,60 +4015,60 @@
       <c r="H38" s="46"/>
     </row>
     <row r="39" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="82" t="s">
+      <c r="A39" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="82"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="83"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83"/>
+      <c r="B39" s="77"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
       <c r="G39" s="21"/>
       <c r="H39" s="46"/>
     </row>
     <row r="40" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="22"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="78"/>
+      <c r="C40" s="83"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
       <c r="H40" s="41"/>
     </row>
     <row r="41" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
       <c r="B41" s="22"/>
-      <c r="C41" s="78"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
+      <c r="C41" s="83"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="83"/>
+      <c r="F41" s="83"/>
+      <c r="G41" s="83"/>
       <c r="H41" s="41"/>
     </row>
     <row r="42" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="81" t="s">
+      <c r="A43" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="81"/>
-      <c r="C43" s="81" t="s">
+      <c r="B43" s="84"/>
+      <c r="C43" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="81"/>
+      <c r="D43" s="84"/>
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
       <c r="G43" s="24"/>
       <c r="H43" s="44"/>
     </row>
     <row r="44" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="85" t="s">
+      <c r="A44" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="85"/>
-      <c r="C44" s="85"/>
-      <c r="D44" s="85"/>
-      <c r="E44" s="85"/>
+      <c r="B44" s="79"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="79"/>
+      <c r="E44" s="79"/>
       <c r="F44" s="39"/>
       <c r="G44" s="3" t="s">
         <v>0</v>
@@ -4089,10 +4083,10 @@
       <c r="C45" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="78"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
-      <c r="G45" s="78"/>
+      <c r="D45" s="83"/>
+      <c r="E45" s="83"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
       <c r="H45" s="40"/>
     </row>
     <row r="46" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4104,9 +4098,9 @@
         <v>23</v>
       </c>
       <c r="D46" s="59"/>
-      <c r="E46" s="78"/>
-      <c r="F46" s="78"/>
-      <c r="G46" s="78"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
       <c r="H46" s="43"/>
     </row>
     <row r="47" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4120,13 +4114,13 @@
       <c r="H47" s="43"/>
     </row>
     <row r="48" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="84" t="s">
+      <c r="A48" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="84"/>
-      <c r="C48" s="84"/>
-      <c r="D48" s="84"/>
-      <c r="E48" s="84"/>
+      <c r="B48" s="80"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="80"/>
       <c r="F48" s="38"/>
       <c r="G48" s="3" t="s">
         <v>25</v>
@@ -4141,9 +4135,9 @@
       <c r="C49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D49" s="86"/>
-      <c r="E49" s="86"/>
-      <c r="F49" s="86"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="81"/>
       <c r="G49" s="3" t="s">
         <v>27</v>
       </c>
@@ -4153,9 +4147,9 @@
       <c r="A50" s="6"/>
       <c r="B50" s="18"/>
       <c r="C50" s="17"/>
-      <c r="D50" s="86"/>
-      <c r="E50" s="86"/>
-      <c r="F50" s="86"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="81"/>
       <c r="G50" s="3" t="s">
         <v>34</v>
       </c>
@@ -4172,43 +4166,43 @@
       <c r="H51" s="46"/>
     </row>
     <row r="52" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="82" t="s">
+      <c r="A52" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="82"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="83"/>
-      <c r="E52" s="83"/>
-      <c r="F52" s="83"/>
+      <c r="B52" s="77"/>
+      <c r="C52" s="77"/>
+      <c r="D52" s="78"/>
+      <c r="E52" s="78"/>
+      <c r="F52" s="78"/>
       <c r="G52" s="21"/>
       <c r="H52" s="46"/>
     </row>
     <row r="53" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="49"/>
       <c r="B53" s="49"/>
-      <c r="C53" s="76"/>
-      <c r="D53" s="76"/>
-      <c r="E53" s="77"/>
-      <c r="F53" s="77"/>
-      <c r="G53" s="77"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="87"/>
+      <c r="F53" s="87"/>
+      <c r="G53" s="87"/>
       <c r="H53" s="50"/>
     </row>
     <row r="54" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22"/>
       <c r="B54" s="22"/>
-      <c r="C54" s="78"/>
-      <c r="D54" s="78"/>
-      <c r="E54" s="78"/>
-      <c r="F54" s="78"/>
-      <c r="G54" s="78"/>
+      <c r="C54" s="83"/>
+      <c r="D54" s="83"/>
+      <c r="E54" s="83"/>
+      <c r="F54" s="83"/>
+      <c r="G54" s="83"/>
       <c r="H54" s="41"/>
     </row>
     <row r="55" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="79"/>
-      <c r="D55" s="79"/>
+      <c r="C55" s="88"/>
+      <c r="D55" s="88"/>
     </row>
     <row r="56" spans="1:8" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27"/>
@@ -4232,27 +4226,27 @@
     </row>
     <row r="58" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="81" t="s">
+      <c r="A59" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B59" s="81"/>
-      <c r="C59" s="81" t="s">
+      <c r="B59" s="84"/>
+      <c r="C59" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="D59" s="81"/>
+      <c r="D59" s="84"/>
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
       <c r="G59" s="24"/>
       <c r="H59" s="44"/>
     </row>
     <row r="60" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="85" t="s">
+      <c r="A60" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="B60" s="85"/>
-      <c r="C60" s="85"/>
-      <c r="D60" s="85"/>
-      <c r="E60" s="85"/>
+      <c r="B60" s="79"/>
+      <c r="C60" s="79"/>
+      <c r="D60" s="79"/>
+      <c r="E60" s="79"/>
       <c r="F60" s="39"/>
       <c r="G60" s="3" t="s">
         <v>0</v>
@@ -4267,10 +4261,10 @@
       <c r="C61" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D61" s="87"/>
-      <c r="E61" s="87"/>
-      <c r="F61" s="87"/>
-      <c r="G61" s="87"/>
+      <c r="D61" s="85"/>
+      <c r="E61" s="85"/>
+      <c r="F61" s="85"/>
+      <c r="G61" s="85"/>
       <c r="H61" s="53"/>
     </row>
     <row r="62" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4282,9 +4276,9 @@
         <v>23</v>
       </c>
       <c r="D62" s="59"/>
-      <c r="E62" s="78"/>
-      <c r="F62" s="78"/>
-      <c r="G62" s="78"/>
+      <c r="E62" s="83"/>
+      <c r="F62" s="83"/>
+      <c r="G62" s="83"/>
       <c r="H62" s="43"/>
     </row>
     <row r="63" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4298,13 +4292,13 @@
       <c r="H63" s="43"/>
     </row>
     <row r="64" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="84" t="s">
+      <c r="A64" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B64" s="84"/>
-      <c r="C64" s="84"/>
-      <c r="D64" s="84"/>
-      <c r="E64" s="84"/>
+      <c r="B64" s="80"/>
+      <c r="C64" s="80"/>
+      <c r="D64" s="80"/>
+      <c r="E64" s="80"/>
       <c r="F64" s="38"/>
       <c r="G64" s="3" t="s">
         <v>25</v>
@@ -4319,9 +4313,9 @@
       <c r="C65" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="78"/>
-      <c r="E65" s="78"/>
-      <c r="F65" s="78"/>
+      <c r="D65" s="83"/>
+      <c r="E65" s="83"/>
+      <c r="F65" s="83"/>
       <c r="G65" s="3" t="s">
         <v>27</v>
       </c>
@@ -4331,9 +4325,9 @@
       <c r="A66" s="6"/>
       <c r="B66" s="18"/>
       <c r="C66" s="17"/>
-      <c r="D66" s="78"/>
-      <c r="E66" s="78"/>
-      <c r="F66" s="78"/>
+      <c r="D66" s="83"/>
+      <c r="E66" s="83"/>
+      <c r="F66" s="83"/>
       <c r="G66" s="3" t="s">
         <v>34</v>
       </c>
@@ -4350,89 +4344,44 @@
       <c r="H67" s="46"/>
     </row>
     <row r="68" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="82" t="s">
+      <c r="A68" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B68" s="82"/>
-      <c r="C68" s="82"/>
-      <c r="D68" s="83"/>
-      <c r="E68" s="83"/>
-      <c r="F68" s="83"/>
+      <c r="B68" s="77"/>
+      <c r="C68" s="77"/>
+      <c r="D68" s="78"/>
+      <c r="E68" s="78"/>
+      <c r="F68" s="78"/>
       <c r="G68" s="21"/>
       <c r="H68" s="46"/>
     </row>
     <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="22"/>
       <c r="B69" s="22"/>
-      <c r="C69" s="78"/>
-      <c r="D69" s="78"/>
-      <c r="E69" s="78"/>
-      <c r="F69" s="78"/>
-      <c r="G69" s="78"/>
+      <c r="C69" s="83"/>
+      <c r="D69" s="83"/>
+      <c r="E69" s="83"/>
+      <c r="F69" s="83"/>
+      <c r="G69" s="83"/>
       <c r="H69" s="41"/>
     </row>
     <row r="70" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="22"/>
       <c r="B70" s="22"/>
-      <c r="C70" s="78"/>
-      <c r="D70" s="78"/>
-      <c r="E70" s="78"/>
-      <c r="F70" s="78"/>
-      <c r="G70" s="78"/>
+      <c r="C70" s="83"/>
+      <c r="D70" s="83"/>
+      <c r="E70" s="83"/>
+      <c r="F70" s="83"/>
+      <c r="G70" s="83"/>
       <c r="H70" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="D36:F37"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="D65:F66"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="A60:E60"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="D49:F50"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="D23:F24"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="A4:B4"/>
@@ -4444,16 +4393,61 @@
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="D10:F11"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="D23:F24"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="D49:F50"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="D65:F66"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="D36:F37"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.57291666666666663" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader xml:space="preserve">&amp;L&amp;"Cambria,Bold"&amp;14Geo Plazas - QUERETARO&amp;12
+    <oddHeader xml:space="preserve">&amp;L&amp;"Cambria,Bold"&amp;14Fundadores - QUERETARO&amp;12
 &amp;R&amp;"Cambria,Bold"&amp;16Programa para la Reunion Publica </oddHeader>
   </headerFooter>
 </worksheet>
@@ -4463,8 +4457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:E40"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4500,22 +4494,18 @@
       <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="90"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="55" t="s">
         <v>44</v>
-      </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="96"/>
-    </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
-        <v>45</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>31</v>
@@ -4527,21 +4517,21 @@
       <c r="E6" s="29"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
-      <c r="B7" s="91" t="s">
+      <c r="A7" s="91"/>
+      <c r="B7" s="93" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="30"/>
-      <c r="D7" s="93" t="s">
+      <c r="D7" s="95" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="30"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="90"/>
-      <c r="B8" s="92"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="31"/>
-      <c r="D8" s="94"/>
+      <c r="D8" s="96"/>
       <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4552,22 +4542,18 @@
       <c r="E9" s="24"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="90"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="55" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="96"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="88" t="s">
-        <v>45</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>31</v>
@@ -4579,40 +4565,36 @@
       <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="89"/>
-      <c r="B15" s="91" t="s">
+      <c r="A15" s="91"/>
+      <c r="B15" s="93" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="30"/>
-      <c r="D15" s="93" t="s">
+      <c r="D15" s="95" t="s">
         <v>32</v>
       </c>
       <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="90"/>
-      <c r="B16" s="92"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="94"/>
       <c r="C16" s="31"/>
-      <c r="D16" s="94"/>
+      <c r="D16" s="96"/>
       <c r="E16" s="31"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="95" t="s">
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="90"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="55" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" s="95"/>
-      <c r="D21" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="96"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="88" t="s">
-        <v>45</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>31</v>
@@ -4624,40 +4606,36 @@
       <c r="E22" s="29"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="89"/>
-      <c r="B23" s="91" t="s">
+      <c r="A23" s="91"/>
+      <c r="B23" s="93" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="30"/>
-      <c r="D23" s="93" t="s">
+      <c r="D23" s="95" t="s">
         <v>32</v>
       </c>
       <c r="E23" s="30"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="90"/>
-      <c r="B24" s="92"/>
+      <c r="A24" s="92"/>
+      <c r="B24" s="94"/>
       <c r="C24" s="31"/>
-      <c r="D24" s="94"/>
+      <c r="D24" s="96"/>
       <c r="E24" s="31"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="95" t="s">
+      <c r="B29" s="89"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="90"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="55" t="s">
         <v>44</v>
-      </c>
-      <c r="C29" s="95"/>
-      <c r="D29" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="E29" s="96"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="88" t="s">
-        <v>45</v>
       </c>
       <c r="B30" s="28" t="s">
         <v>31</v>
@@ -4669,40 +4647,36 @@
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="89"/>
-      <c r="B31" s="91" t="s">
+      <c r="A31" s="91"/>
+      <c r="B31" s="93" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="30"/>
-      <c r="D31" s="93" t="s">
+      <c r="D31" s="95" t="s">
         <v>32</v>
       </c>
       <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="90"/>
-      <c r="B32" s="92"/>
+      <c r="A32" s="92"/>
+      <c r="B32" s="94"/>
       <c r="C32" s="31"/>
-      <c r="D32" s="94"/>
+      <c r="D32" s="96"/>
       <c r="E32" s="31"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="95" t="s">
+      <c r="B37" s="89"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="90"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="55" t="s">
         <v>44</v>
-      </c>
-      <c r="C37" s="95"/>
-      <c r="D37" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="96"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="88" t="s">
-        <v>45</v>
       </c>
       <c r="B38" s="28" t="s">
         <v>31</v>
@@ -4714,55 +4688,55 @@
       <c r="E38" s="29"/>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="89"/>
-      <c r="B39" s="91" t="s">
+      <c r="A39" s="91"/>
+      <c r="B39" s="93" t="s">
         <v>32</v>
       </c>
       <c r="C39" s="30"/>
-      <c r="D39" s="93" t="s">
+      <c r="D39" s="95" t="s">
         <v>32</v>
       </c>
       <c r="E39" s="30"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="90"/>
-      <c r="B40" s="92"/>
+      <c r="A40" s="92"/>
+      <c r="B40" s="94"/>
       <c r="C40" s="31"/>
-      <c r="D40" s="94"/>
+      <c r="D40" s="96"/>
       <c r="E40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Cambria,Bold"&amp;14Geo Plazas - QUERETARO&amp;"-,Regular"
+    <oddHeader>&amp;L&amp;"Cambria,Bold"&amp;14Fundadores - QUERETARO&amp;"-,Regular"
 &amp;R&amp;"Cambria,Bold"&amp;16Programa de Acomodadores</oddHeader>
   </headerFooter>
 </worksheet>

</xml_diff>

<commit_message>
Commit End Week 1905 update on DB,pending Time
</commit_message>
<xml_diff>
--- a/Project_Insight/bin/Debug/Programs.xlsx
+++ b/Project_Insight/bin/Debug/Programs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13545" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13545"/>
   </bookViews>
   <sheets>
     <sheet name="VyM" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="45">
   <si>
     <t>Presidente:</t>
   </si>
@@ -282,7 +282,7 @@
     <t xml:space="preserve"> (10 mins.)</t>
   </si>
   <si>
-    <t>Aseo:</t>
+    <t>Encargado Aseo:</t>
   </si>
 </sst>
 </file>
@@ -797,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -888,9 +888,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -944,68 +941,92 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1013,59 +1034,41 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1356,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127:F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,22 +1393,22 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
       <c r="F3" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="65"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
       <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1418,11 +1421,11 @@
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
       <c r="F5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1435,13 +1438,13 @@
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -1453,13 +1456,13 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
         <v>9</v>
@@ -1472,12 +1475,12 @@
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1487,12 +1490,12 @@
       <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1526,71 +1529,71 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>0.31388888888888888</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="51"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="50"/>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>0.31666666666666665</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>0.31944444444444448</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
     </row>
-    <row r="17" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
       <c r="F17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1599,13 +1602,13 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
@@ -1616,11 +1619,11 @@
       <c r="B19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
       <c r="F19" s="2"/>
       <c r="G19" s="14"/>
     </row>
@@ -1631,45 +1634,45 @@
       <c r="B20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="70">
+      <c r="A22" s="74">
         <v>0.33819444444444446</v>
       </c>
-      <c r="B22" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="56" t="s">
+      <c r="B22" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
       <c r="F22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="70"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
+      <c r="A23" s="74"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
       <c r="F23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1682,12 +1685,12 @@
       <c r="B24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="56" t="s">
+      <c r="C24" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1707,7 +1710,7 @@
       </c>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1728,22 +1731,22 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="63"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
       <c r="F28" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G28" s="34"/>
     </row>
     <row r="29" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
       <c r="F29" s="3" t="s">
         <v>1</v>
       </c>
@@ -1756,11 +1759,11 @@
       <c r="B30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="59" t="s">
+      <c r="C30" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
       <c r="F30" s="3" t="s">
         <v>2</v>
       </c>
@@ -1773,13 +1776,13 @@
       <c r="B31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="59" t="s">
+      <c r="C31" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
     </row>
     <row r="32" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
@@ -1791,13 +1794,13 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="67"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4" t="s">
         <v>9</v>
@@ -1810,12 +1813,12 @@
       <c r="B34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="62" t="s">
+      <c r="C34" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
       <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1825,12 +1828,12 @@
       <c r="B35" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="59" t="s">
+      <c r="C35" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="59"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
       <c r="G35" s="12"/>
     </row>
     <row r="36" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1864,71 +1867,71 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="60" t="s">
+      <c r="A38" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="61"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="61"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>0.31388888888888888</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="56" t="s">
+      <c r="C39" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="51"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="50"/>
       <c r="G39" s="13"/>
     </row>
-    <row r="40" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>0.31666666666666665</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="56" t="s">
+      <c r="C40" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
     </row>
-    <row r="41" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>0.31944444444444448</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="56" t="s">
+      <c r="C41" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
     </row>
-    <row r="42" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
       <c r="F42" s="2" t="s">
         <v>33</v>
       </c>
@@ -1937,13 +1940,13 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="57" t="s">
+      <c r="A43" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B43" s="58"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
@@ -1951,14 +1954,14 @@
       <c r="A44" s="6">
         <v>0.32500000000000001</v>
       </c>
-      <c r="B44" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="59" t="s">
+      <c r="B44" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
       <c r="F44" s="2"/>
       <c r="G44" s="14"/>
     </row>
@@ -1966,49 +1969,49 @@
       <c r="A45" s="6">
         <v>0.32708333333333334</v>
       </c>
-      <c r="B45" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="56" t="s">
+      <c r="B45" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
       <c r="G45" s="12"/>
     </row>
     <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
-      <c r="B46" s="54"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="52"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="51"/>
     </row>
     <row r="47" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="70">
+      <c r="A47" s="74">
         <v>0.33819444444444446</v>
       </c>
-      <c r="B47" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="56" t="s">
+      <c r="B47" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
       <c r="F47" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G47" s="12"/>
     </row>
     <row r="48" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="70"/>
-      <c r="B48" s="69"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
+      <c r="A48" s="74"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
       <c r="F48" s="3" t="s">
         <v>27</v>
       </c>
@@ -2018,22 +2021,22 @@
       <c r="A49" s="6">
         <v>0.35902777777777778</v>
       </c>
-      <c r="B49" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" s="56" t="s">
+      <c r="B49" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
       <c r="G49" s="14"/>
     </row>
     <row r="50" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>0.3611111111111111</v>
       </c>
-      <c r="B50" s="54" t="s">
+      <c r="B50" s="53" t="s">
         <v>4</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -2046,7 +2049,7 @@
       </c>
       <c r="G50" s="12"/>
     </row>
-    <row r="51" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2065,14 +2068,14 @@
       <c r="G52" s="9"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="75" t="s">
+      <c r="A53" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="75"/>
-      <c r="C53" s="75"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="76"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="66"/>
       <c r="G53" s="10" t="s">
         <v>14</v>
       </c>
@@ -2096,22 +2099,22 @@
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="63"/>
-      <c r="B56" s="63"/>
-      <c r="C56" s="64"/>
-      <c r="D56" s="63"/>
-      <c r="E56" s="63"/>
+      <c r="A56" s="61"/>
+      <c r="B56" s="61"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="61"/>
+      <c r="E56" s="61"/>
       <c r="F56" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G56" s="34"/>
     </row>
     <row r="57" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="65"/>
-      <c r="B57" s="65"/>
-      <c r="C57" s="66"/>
-      <c r="D57" s="65"/>
-      <c r="E57" s="65"/>
+      <c r="A57" s="62"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
       <c r="F57" s="3" t="s">
         <v>1</v>
       </c>
@@ -2124,11 +2127,11 @@
       <c r="B58" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="59" t="s">
+      <c r="C58" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="71"/>
       <c r="F58" s="3" t="s">
         <v>2</v>
       </c>
@@ -2141,13 +2144,13 @@
       <c r="B59" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="59" t="s">
+      <c r="C59" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="59"/>
-      <c r="E59" s="59"/>
-      <c r="F59" s="59"/>
-      <c r="G59" s="59"/>
+      <c r="D59" s="71"/>
+      <c r="E59" s="71"/>
+      <c r="F59" s="71"/>
+      <c r="G59" s="71"/>
     </row>
     <row r="60" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
@@ -2159,13 +2162,13 @@
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="67" t="s">
+      <c r="A61" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="67"/>
-      <c r="C61" s="68"/>
-      <c r="D61" s="68"/>
-      <c r="E61" s="68"/>
+      <c r="B61" s="75"/>
+      <c r="C61" s="76"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="76"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4" t="s">
         <v>9</v>
@@ -2178,12 +2181,12 @@
       <c r="B62" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="62" t="s">
+      <c r="C62" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="D62" s="56"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="56"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="57"/>
+      <c r="F62" s="57"/>
       <c r="G62" s="12"/>
     </row>
     <row r="63" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2193,12 +2196,12 @@
       <c r="B63" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C63" s="59" t="s">
+      <c r="C63" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="D63" s="59"/>
-      <c r="E63" s="59"/>
-      <c r="F63" s="59"/>
+      <c r="D63" s="71"/>
+      <c r="E63" s="71"/>
+      <c r="F63" s="71"/>
       <c r="G63" s="12"/>
     </row>
     <row r="64" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2232,71 +2235,71 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="60" t="s">
+      <c r="A66" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="61"/>
-      <c r="C66" s="61"/>
-      <c r="D66" s="61"/>
-      <c r="E66" s="61"/>
+      <c r="B66" s="59"/>
+      <c r="C66" s="59"/>
+      <c r="D66" s="59"/>
+      <c r="E66" s="59"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>0.31388888888888888</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="56" t="s">
+      <c r="C67" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D67" s="56"/>
-      <c r="E67" s="56"/>
-      <c r="F67" s="51"/>
+      <c r="D67" s="57"/>
+      <c r="E67" s="57"/>
+      <c r="F67" s="50"/>
       <c r="G67" s="13"/>
     </row>
-    <row r="68" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>0.31666666666666665</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="56" t="s">
+      <c r="C68" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="56"/>
-      <c r="E68" s="56"/>
+      <c r="D68" s="57"/>
+      <c r="E68" s="57"/>
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
     </row>
-    <row r="69" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>0.31944444444444448</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="56" t="s">
+      <c r="C69" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D69" s="56"/>
-      <c r="E69" s="56"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="57"/>
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
     </row>
-    <row r="70" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
+      <c r="D70" s="71"/>
+      <c r="E70" s="71"/>
       <c r="F70" s="2" t="s">
         <v>33</v>
       </c>
@@ -2305,13 +2308,13 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="57" t="s">
+      <c r="A71" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B71" s="58"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="58"/>
-      <c r="E71" s="58"/>
+      <c r="B71" s="73"/>
+      <c r="C71" s="73"/>
+      <c r="D71" s="73"/>
+      <c r="E71" s="73"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
     </row>
@@ -2319,14 +2322,14 @@
       <c r="A72" s="6">
         <v>0.32500000000000001</v>
       </c>
-      <c r="B72" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C72" s="59" t="s">
+      <c r="B72" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D72" s="59"/>
-      <c r="E72" s="59"/>
+      <c r="D72" s="71"/>
+      <c r="E72" s="71"/>
       <c r="F72" s="2"/>
       <c r="G72" s="14"/>
     </row>
@@ -2334,49 +2337,49 @@
       <c r="A73" s="6">
         <v>0.32708333333333334</v>
       </c>
-      <c r="B73" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C73" s="56" t="s">
+      <c r="B73" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="56"/>
-      <c r="E73" s="56"/>
-      <c r="F73" s="56"/>
+      <c r="D73" s="57"/>
+      <c r="E73" s="57"/>
+      <c r="F73" s="57"/>
       <c r="G73" s="12"/>
     </row>
     <row r="74" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
-      <c r="B74" s="54"/>
-      <c r="C74" s="56"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="56"/>
-      <c r="G74" s="52"/>
+      <c r="B74" s="53"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="57"/>
+      <c r="E74" s="57"/>
+      <c r="F74" s="57"/>
+      <c r="G74" s="51"/>
     </row>
     <row r="75" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="70">
+      <c r="A75" s="74">
         <v>0.33819444444444446</v>
       </c>
-      <c r="B75" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75" s="56" t="s">
+      <c r="B75" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D75" s="56"/>
-      <c r="E75" s="56"/>
+      <c r="D75" s="57"/>
+      <c r="E75" s="57"/>
       <c r="F75" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G75" s="12"/>
     </row>
     <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="70"/>
-      <c r="B76" s="69"/>
-      <c r="C76" s="56"/>
-      <c r="D76" s="56"/>
-      <c r="E76" s="56"/>
+      <c r="A76" s="74"/>
+      <c r="B76" s="60"/>
+      <c r="C76" s="57"/>
+      <c r="D76" s="57"/>
+      <c r="E76" s="57"/>
       <c r="F76" s="3" t="s">
         <v>27</v>
       </c>
@@ -2386,22 +2389,22 @@
       <c r="A77" s="6">
         <v>0.35902777777777778</v>
       </c>
-      <c r="B77" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C77" s="56" t="s">
+      <c r="B77" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D77" s="56"/>
-      <c r="E77" s="56"/>
-      <c r="F77" s="56"/>
+      <c r="D77" s="57"/>
+      <c r="E77" s="57"/>
+      <c r="F77" s="57"/>
       <c r="G77" s="14"/>
     </row>
     <row r="78" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
         <v>0.3611111111111111</v>
       </c>
-      <c r="B78" s="54" t="s">
+      <c r="B78" s="53" t="s">
         <v>4</v>
       </c>
       <c r="C78" s="2" t="s">
@@ -2414,7 +2417,7 @@
       </c>
       <c r="G78" s="12"/>
     </row>
-    <row r="79" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2433,22 +2436,22 @@
       <c r="G80" s="2"/>
     </row>
     <row r="81" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="63"/>
-      <c r="B81" s="63"/>
-      <c r="C81" s="64"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="63"/>
+      <c r="A81" s="61"/>
+      <c r="B81" s="61"/>
+      <c r="C81" s="63"/>
+      <c r="D81" s="61"/>
+      <c r="E81" s="61"/>
       <c r="F81" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G81" s="34"/>
     </row>
     <row r="82" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="65"/>
-      <c r="B82" s="65"/>
-      <c r="C82" s="66"/>
-      <c r="D82" s="65"/>
-      <c r="E82" s="65"/>
+      <c r="A82" s="62"/>
+      <c r="B82" s="62"/>
+      <c r="C82" s="64"/>
+      <c r="D82" s="62"/>
+      <c r="E82" s="62"/>
       <c r="F82" s="3" t="s">
         <v>1</v>
       </c>
@@ -2461,11 +2464,11 @@
       <c r="B83" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C83" s="59" t="s">
+      <c r="C83" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="D83" s="59"/>
-      <c r="E83" s="59"/>
+      <c r="D83" s="71"/>
+      <c r="E83" s="71"/>
       <c r="F83" s="3" t="s">
         <v>2</v>
       </c>
@@ -2478,13 +2481,13 @@
       <c r="B84" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C84" s="59" t="s">
+      <c r="C84" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="D84" s="59"/>
-      <c r="E84" s="59"/>
-      <c r="F84" s="59"/>
-      <c r="G84" s="59"/>
+      <c r="D84" s="71"/>
+      <c r="E84" s="71"/>
+      <c r="F84" s="71"/>
+      <c r="G84" s="71"/>
     </row>
     <row r="85" spans="1:7" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
@@ -2496,13 +2499,13 @@
       <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="67" t="s">
+      <c r="A86" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B86" s="67"/>
-      <c r="C86" s="68"/>
-      <c r="D86" s="68"/>
-      <c r="E86" s="68"/>
+      <c r="B86" s="75"/>
+      <c r="C86" s="76"/>
+      <c r="D86" s="76"/>
+      <c r="E86" s="76"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4" t="s">
         <v>9</v>
@@ -2515,12 +2518,12 @@
       <c r="B87" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="62" t="s">
+      <c r="C87" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="D87" s="56"/>
-      <c r="E87" s="56"/>
-      <c r="F87" s="56"/>
+      <c r="D87" s="57"/>
+      <c r="E87" s="57"/>
+      <c r="F87" s="57"/>
       <c r="G87" s="12"/>
     </row>
     <row r="88" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2530,12 +2533,12 @@
       <c r="B88" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C88" s="59" t="s">
+      <c r="C88" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="D88" s="59"/>
-      <c r="E88" s="59"/>
-      <c r="F88" s="59"/>
+      <c r="D88" s="71"/>
+      <c r="E88" s="71"/>
+      <c r="F88" s="71"/>
       <c r="G88" s="12"/>
     </row>
     <row r="89" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2569,71 +2572,71 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="60" t="s">
+      <c r="A91" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="61"/>
-      <c r="C91" s="61"/>
-      <c r="D91" s="61"/>
-      <c r="E91" s="61"/>
+      <c r="B91" s="59"/>
+      <c r="C91" s="59"/>
+      <c r="D91" s="59"/>
+      <c r="E91" s="59"/>
       <c r="F91" s="4"/>
       <c r="G91" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
         <v>0.31388888888888888</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C92" s="56" t="s">
+      <c r="C92" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D92" s="56"/>
-      <c r="E92" s="56"/>
-      <c r="F92" s="51"/>
+      <c r="D92" s="57"/>
+      <c r="E92" s="57"/>
+      <c r="F92" s="50"/>
       <c r="G92" s="13"/>
     </row>
-    <row r="93" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
         <v>0.31666666666666665</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C93" s="56" t="s">
+      <c r="C93" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="D93" s="56"/>
-      <c r="E93" s="56"/>
+      <c r="D93" s="57"/>
+      <c r="E93" s="57"/>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
     </row>
-    <row r="94" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>0.31944444444444448</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C94" s="56" t="s">
+      <c r="C94" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D94" s="56"/>
-      <c r="E94" s="56"/>
+      <c r="D94" s="57"/>
+      <c r="E94" s="57"/>
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
     </row>
-    <row r="95" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
+      <c r="D95" s="71"/>
+      <c r="E95" s="71"/>
       <c r="F95" s="2" t="s">
         <v>33</v>
       </c>
@@ -2642,13 +2645,13 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="57" t="s">
+      <c r="A96" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B96" s="58"/>
-      <c r="C96" s="58"/>
-      <c r="D96" s="58"/>
-      <c r="E96" s="58"/>
+      <c r="B96" s="73"/>
+      <c r="C96" s="73"/>
+      <c r="D96" s="73"/>
+      <c r="E96" s="73"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
     </row>
@@ -2656,14 +2659,14 @@
       <c r="A97" s="6">
         <v>0.32500000000000001</v>
       </c>
-      <c r="B97" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C97" s="59" t="s">
+      <c r="B97" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D97" s="59"/>
-      <c r="E97" s="59"/>
+      <c r="D97" s="71"/>
+      <c r="E97" s="71"/>
       <c r="F97" s="2"/>
       <c r="G97" s="14"/>
     </row>
@@ -2671,49 +2674,49 @@
       <c r="A98" s="6">
         <v>0.32708333333333334</v>
       </c>
-      <c r="B98" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C98" s="56" t="s">
+      <c r="B98" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D98" s="56"/>
-      <c r="E98" s="56"/>
-      <c r="F98" s="56"/>
+      <c r="D98" s="57"/>
+      <c r="E98" s="57"/>
+      <c r="F98" s="57"/>
       <c r="G98" s="12"/>
     </row>
     <row r="99" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
-      <c r="B99" s="54"/>
-      <c r="C99" s="56"/>
-      <c r="D99" s="56"/>
-      <c r="E99" s="56"/>
-      <c r="F99" s="56"/>
-      <c r="G99" s="52"/>
+      <c r="B99" s="53"/>
+      <c r="C99" s="57"/>
+      <c r="D99" s="57"/>
+      <c r="E99" s="57"/>
+      <c r="F99" s="57"/>
+      <c r="G99" s="51"/>
     </row>
     <row r="100" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="70">
+      <c r="A100" s="74">
         <v>0.33819444444444446</v>
       </c>
-      <c r="B100" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C100" s="56" t="s">
+      <c r="B100" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D100" s="56"/>
-      <c r="E100" s="56"/>
+      <c r="D100" s="57"/>
+      <c r="E100" s="57"/>
       <c r="F100" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G100" s="12"/>
     </row>
     <row r="101" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="70"/>
-      <c r="B101" s="69"/>
-      <c r="C101" s="56"/>
-      <c r="D101" s="56"/>
-      <c r="E101" s="56"/>
+      <c r="A101" s="74"/>
+      <c r="B101" s="60"/>
+      <c r="C101" s="57"/>
+      <c r="D101" s="57"/>
+      <c r="E101" s="57"/>
       <c r="F101" s="3" t="s">
         <v>27</v>
       </c>
@@ -2723,22 +2726,22 @@
       <c r="A102" s="6">
         <v>0.35902777777777778</v>
       </c>
-      <c r="B102" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C102" s="56" t="s">
+      <c r="B102" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C102" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D102" s="56"/>
-      <c r="E102" s="56"/>
-      <c r="F102" s="56"/>
+      <c r="D102" s="57"/>
+      <c r="E102" s="57"/>
+      <c r="F102" s="57"/>
       <c r="G102" s="14"/>
     </row>
     <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>0.3611111111111111</v>
       </c>
-      <c r="B103" s="54" t="s">
+      <c r="B103" s="53" t="s">
         <v>4</v>
       </c>
       <c r="C103" s="2" t="s">
@@ -2751,7 +2754,7 @@
       </c>
       <c r="G103" s="12"/>
     </row>
-    <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2770,12 +2773,12 @@
       <c r="G105" s="9"/>
     </row>
     <row r="106" spans="1:7" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="73"/>
-      <c r="B106" s="73"/>
-      <c r="C106" s="73"/>
-      <c r="D106" s="73"/>
-      <c r="E106" s="73"/>
-      <c r="F106" s="74"/>
+      <c r="A106" s="69"/>
+      <c r="B106" s="69"/>
+      <c r="C106" s="69"/>
+      <c r="D106" s="69"/>
+      <c r="E106" s="69"/>
+      <c r="F106" s="70"/>
       <c r="G106" s="10" t="s">
         <v>15</v>
       </c>
@@ -2799,22 +2802,22 @@
       <c r="G108" s="2"/>
     </row>
     <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="63"/>
-      <c r="B109" s="63"/>
-      <c r="C109" s="64"/>
-      <c r="D109" s="63"/>
-      <c r="E109" s="63"/>
+      <c r="A109" s="61"/>
+      <c r="B109" s="61"/>
+      <c r="C109" s="63"/>
+      <c r="D109" s="61"/>
+      <c r="E109" s="61"/>
       <c r="F109" s="25" t="s">
         <v>0</v>
       </c>
       <c r="G109" s="34"/>
     </row>
     <row r="110" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="65"/>
-      <c r="B110" s="65"/>
-      <c r="C110" s="66"/>
-      <c r="D110" s="65"/>
-      <c r="E110" s="65"/>
+      <c r="A110" s="62"/>
+      <c r="B110" s="62"/>
+      <c r="C110" s="64"/>
+      <c r="D110" s="62"/>
+      <c r="E110" s="62"/>
       <c r="F110" s="3" t="s">
         <v>1</v>
       </c>
@@ -2827,11 +2830,11 @@
       <c r="B111" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C111" s="59" t="s">
+      <c r="C111" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="D111" s="59"/>
-      <c r="E111" s="59"/>
+      <c r="D111" s="71"/>
+      <c r="E111" s="71"/>
       <c r="F111" s="3" t="s">
         <v>2</v>
       </c>
@@ -2844,13 +2847,13 @@
       <c r="B112" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C112" s="59" t="s">
+      <c r="C112" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="D112" s="59"/>
-      <c r="E112" s="59"/>
-      <c r="F112" s="59"/>
-      <c r="G112" s="59"/>
+      <c r="D112" s="71"/>
+      <c r="E112" s="71"/>
+      <c r="F112" s="71"/>
+      <c r="G112" s="71"/>
     </row>
     <row r="113" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
@@ -2862,13 +2865,13 @@
       <c r="G113" s="2"/>
     </row>
     <row r="114" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="67" t="s">
+      <c r="A114" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B114" s="67"/>
-      <c r="C114" s="68"/>
-      <c r="D114" s="68"/>
-      <c r="E114" s="68"/>
+      <c r="B114" s="75"/>
+      <c r="C114" s="76"/>
+      <c r="D114" s="76"/>
+      <c r="E114" s="76"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4" t="s">
         <v>9</v>
@@ -2881,12 +2884,12 @@
       <c r="B115" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C115" s="62" t="s">
+      <c r="C115" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="D115" s="56"/>
-      <c r="E115" s="56"/>
-      <c r="F115" s="56"/>
+      <c r="D115" s="57"/>
+      <c r="E115" s="57"/>
+      <c r="F115" s="57"/>
       <c r="G115" s="12"/>
     </row>
     <row r="116" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2896,12 +2899,12 @@
       <c r="B116" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C116" s="59" t="s">
+      <c r="C116" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="D116" s="59"/>
-      <c r="E116" s="59"/>
-      <c r="F116" s="59"/>
+      <c r="D116" s="71"/>
+      <c r="E116" s="71"/>
+      <c r="F116" s="71"/>
       <c r="G116" s="12"/>
     </row>
     <row r="117" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2935,71 +2938,71 @@
       </c>
     </row>
     <row r="119" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="60" t="s">
+      <c r="A119" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B119" s="61"/>
-      <c r="C119" s="61"/>
-      <c r="D119" s="61"/>
-      <c r="E119" s="61"/>
+      <c r="B119" s="59"/>
+      <c r="C119" s="59"/>
+      <c r="D119" s="59"/>
+      <c r="E119" s="59"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6">
         <v>0.31388888888888888</v>
       </c>
       <c r="B120" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C120" s="56" t="s">
+      <c r="C120" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D120" s="56"/>
-      <c r="E120" s="56"/>
-      <c r="F120" s="51"/>
+      <c r="D120" s="57"/>
+      <c r="E120" s="57"/>
+      <c r="F120" s="50"/>
       <c r="G120" s="13"/>
     </row>
-    <row r="121" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6">
         <v>0.31666666666666665</v>
       </c>
       <c r="B121" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C121" s="56" t="s">
+      <c r="C121" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="D121" s="56"/>
-      <c r="E121" s="56"/>
+      <c r="D121" s="57"/>
+      <c r="E121" s="57"/>
       <c r="F121" s="13"/>
       <c r="G121" s="13"/>
     </row>
-    <row r="122" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6">
         <v>0.31944444444444448</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C122" s="56" t="s">
+      <c r="C122" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="D122" s="56"/>
-      <c r="E122" s="56"/>
+      <c r="D122" s="57"/>
+      <c r="E122" s="57"/>
       <c r="F122" s="13"/>
       <c r="G122" s="13"/>
     </row>
     <row r="123" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="D123" s="2"/>
-      <c r="E123" s="2"/>
+      <c r="D123" s="71"/>
+      <c r="E123" s="71"/>
       <c r="F123" s="2" t="s">
         <v>33</v>
       </c>
@@ -3008,13 +3011,13 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="57" t="s">
+      <c r="A124" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B124" s="58"/>
-      <c r="C124" s="58"/>
-      <c r="D124" s="58"/>
-      <c r="E124" s="58"/>
+      <c r="B124" s="73"/>
+      <c r="C124" s="73"/>
+      <c r="D124" s="73"/>
+      <c r="E124" s="73"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
     </row>
@@ -3022,14 +3025,14 @@
       <c r="A125" s="6">
         <v>0.32500000000000001</v>
       </c>
-      <c r="B125" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C125" s="59" t="s">
+      <c r="B125" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C125" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D125" s="59"/>
-      <c r="E125" s="59"/>
+      <c r="D125" s="71"/>
+      <c r="E125" s="71"/>
       <c r="F125" s="2"/>
       <c r="G125" s="14"/>
     </row>
@@ -3037,49 +3040,49 @@
       <c r="A126" s="6">
         <v>0.32708333333333334</v>
       </c>
-      <c r="B126" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C126" s="56" t="s">
+      <c r="B126" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D126" s="56"/>
-      <c r="E126" s="56"/>
-      <c r="F126" s="56"/>
+      <c r="D126" s="57"/>
+      <c r="E126" s="57"/>
+      <c r="F126" s="57"/>
       <c r="G126" s="12"/>
     </row>
     <row r="127" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6"/>
-      <c r="B127" s="54"/>
-      <c r="C127" s="56"/>
-      <c r="D127" s="56"/>
-      <c r="E127" s="56"/>
-      <c r="F127" s="56"/>
-      <c r="G127" s="52"/>
+      <c r="B127" s="53"/>
+      <c r="C127" s="57"/>
+      <c r="D127" s="57"/>
+      <c r="E127" s="57"/>
+      <c r="F127" s="57"/>
+      <c r="G127" s="51"/>
     </row>
     <row r="128" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="70">
+      <c r="A128" s="74">
         <v>0.33819444444444446</v>
       </c>
-      <c r="B128" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C128" s="56" t="s">
+      <c r="B128" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D128" s="56"/>
-      <c r="E128" s="56"/>
+      <c r="D128" s="57"/>
+      <c r="E128" s="57"/>
       <c r="F128" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G128" s="12"/>
     </row>
     <row r="129" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="70"/>
-      <c r="B129" s="69"/>
-      <c r="C129" s="56"/>
-      <c r="D129" s="56"/>
-      <c r="E129" s="56"/>
+      <c r="A129" s="74"/>
+      <c r="B129" s="60"/>
+      <c r="C129" s="57"/>
+      <c r="D129" s="57"/>
+      <c r="E129" s="57"/>
       <c r="F129" s="3" t="s">
         <v>27</v>
       </c>
@@ -3089,22 +3092,22 @@
       <c r="A130" s="6">
         <v>0.35902777777777778</v>
       </c>
-      <c r="B130" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C130" s="56" t="s">
+      <c r="B130" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C130" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="D130" s="56"/>
-      <c r="E130" s="56"/>
-      <c r="F130" s="56"/>
+      <c r="D130" s="57"/>
+      <c r="E130" s="57"/>
+      <c r="F130" s="57"/>
       <c r="G130" s="14"/>
     </row>
     <row r="131" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6">
         <v>0.3611111111111111</v>
       </c>
-      <c r="B131" s="54" t="s">
+      <c r="B131" s="53" t="s">
         <v>4</v>
       </c>
       <c r="C131" s="2" t="s">
@@ -3343,12 +3346,12 @@
       <c r="G156" s="2"/>
     </row>
     <row r="157" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="71"/>
-      <c r="B157" s="71"/>
-      <c r="C157" s="71"/>
-      <c r="D157" s="71"/>
-      <c r="E157" s="71"/>
-      <c r="F157" s="72"/>
+      <c r="A157" s="67"/>
+      <c r="B157" s="67"/>
+      <c r="C157" s="67"/>
+      <c r="D157" s="67"/>
+      <c r="E157" s="67"/>
+      <c r="F157" s="68"/>
       <c r="G157" s="10" t="s">
         <v>16</v>
       </c>
@@ -3426,21 +3429,70 @@
       <c r="G165" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="98">
+  <mergeCells count="103">
+    <mergeCell ref="C126:F126"/>
+    <mergeCell ref="A124:E124"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="A119:E119"/>
+    <mergeCell ref="C120:E120"/>
     <mergeCell ref="D109:E110"/>
+    <mergeCell ref="C115:F115"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="C99:F99"/>
+    <mergeCell ref="C77:F77"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C87:F87"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C111:E111"/>
+    <mergeCell ref="A81:C82"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C88:F88"/>
+    <mergeCell ref="A109:C110"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A86:E86"/>
+    <mergeCell ref="C75:E76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A71:E71"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:E48"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="D81:E82"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
     <mergeCell ref="D3:E4"/>
     <mergeCell ref="A3:C4"/>
     <mergeCell ref="A28:C29"/>
     <mergeCell ref="D28:E29"/>
     <mergeCell ref="A56:C57"/>
     <mergeCell ref="D56:E57"/>
-    <mergeCell ref="C72:E72"/>
     <mergeCell ref="C49:F49"/>
     <mergeCell ref="A53:F53"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="A66:E66"/>
     <mergeCell ref="A157:F157"/>
     <mergeCell ref="C94:E94"/>
     <mergeCell ref="A106:F106"/>
@@ -3457,8 +3509,15 @@
     <mergeCell ref="C127:F127"/>
     <mergeCell ref="C112:G112"/>
     <mergeCell ref="A114:E114"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="A66:E66"/>
     <mergeCell ref="C22:E23"/>
     <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C42:E42"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="C59:G59"/>
     <mergeCell ref="C63:F63"/>
@@ -3473,58 +3532,7 @@
     <mergeCell ref="A61:E61"/>
     <mergeCell ref="C62:F62"/>
     <mergeCell ref="A47:A48"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
     <mergeCell ref="A38:E38"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A86:E86"/>
-    <mergeCell ref="C75:E76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A71:E71"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:E48"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="D81:E82"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C115:F115"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="C99:F99"/>
-    <mergeCell ref="C77:F77"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C87:F87"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C111:E111"/>
-    <mergeCell ref="A81:C82"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C88:F88"/>
-    <mergeCell ref="A109:C110"/>
-    <mergeCell ref="C126:F126"/>
-    <mergeCell ref="A124:E124"/>
-    <mergeCell ref="C125:E125"/>
-    <mergeCell ref="C116:F116"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="A119:E119"/>
-    <mergeCell ref="C120:E120"/>
   </mergeCells>
   <pageMargins left="0.79" right="0.75" top="0.58333333333333337" bottom="0.4375" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3553,7 +3561,7 @@
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" style="47" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3564,7 +3572,7 @@
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
-      <c r="H1" s="42"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
@@ -3574,7 +3582,7 @@
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
-      <c r="H2" s="46"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -3584,35 +3592,35 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="43"/>
+      <c r="H3" s="42"/>
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84" t="s">
+      <c r="B4" s="83"/>
+      <c r="C4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="24"/>
-      <c r="H4" s="44"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="39"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="38"/>
       <c r="G5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="40"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
@@ -3622,25 +3630,25 @@
       <c r="C6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="40"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="39"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="43"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -3650,21 +3658,21 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="43"/>
+      <c r="H8" s="42"/>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="45"/>
+      <c r="H9" s="44"/>
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -3674,25 +3682,25 @@
       <c r="C10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
       <c r="G10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="45"/>
+      <c r="H10" s="44"/>
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="18"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
       <c r="G11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="45"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
@@ -3702,19 +3710,19 @@
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="46"/>
+      <c r="H12" s="45"/>
     </row>
     <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
       <c r="G13" s="21"/>
-      <c r="H13" s="46"/>
+      <c r="H13" s="45"/>
     </row>
     <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
@@ -3724,7 +3732,7 @@
       <c r="E14" s="82"/>
       <c r="F14" s="82"/>
       <c r="G14" s="82"/>
-      <c r="H14" s="41"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
@@ -3738,36 +3746,36 @@
       </c>
       <c r="F15" s="82"/>
       <c r="G15" s="82"/>
-      <c r="H15" s="41"/>
+      <c r="H15" s="40"/>
     </row>
     <row r="16" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="84" t="s">
+      <c r="A17" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84" t="s">
+      <c r="B17" s="83"/>
+      <c r="C17" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="84"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="24"/>
-      <c r="H17" s="44"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="79" t="s">
+      <c r="A18" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="39"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H18" s="40"/>
+      <c r="H18" s="39"/>
     </row>
     <row r="19" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
@@ -3777,25 +3785,25 @@
       <c r="C19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="83"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="83"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="40"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="39"/>
     </row>
     <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="59" t="s">
+      <c r="C20" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="43"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="42"/>
     </row>
     <row r="21" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -3805,21 +3813,21 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="43"/>
+      <c r="H21" s="42"/>
     </row>
     <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="38"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="37"/>
       <c r="G22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="45"/>
+      <c r="H22" s="44"/>
     </row>
     <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
@@ -3829,25 +3837,25 @@
       <c r="C23" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
       <c r="G23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="45"/>
+      <c r="H23" s="44"/>
     </row>
     <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="18"/>
       <c r="C24" s="17"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
       <c r="G24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="45"/>
+      <c r="H24" s="44"/>
     </row>
     <row r="25" spans="1:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
@@ -3857,19 +3865,19 @@
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
-      <c r="H25" s="46"/>
+      <c r="H25" s="45"/>
     </row>
     <row r="26" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="77"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
       <c r="G26" s="21"/>
-      <c r="H26" s="46"/>
+      <c r="H26" s="45"/>
     </row>
     <row r="27" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
@@ -3879,7 +3887,7 @@
       <c r="E27" s="82"/>
       <c r="F27" s="82"/>
       <c r="G27" s="82"/>
-      <c r="H27" s="41"/>
+      <c r="H27" s="40"/>
     </row>
     <row r="28" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
@@ -3893,36 +3901,36 @@
       </c>
       <c r="F28" s="82"/>
       <c r="G28" s="82"/>
-      <c r="H28" s="41"/>
+      <c r="H28" s="40"/>
     </row>
     <row r="29" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="84" t="s">
+      <c r="A30" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84" t="s">
+      <c r="B30" s="83"/>
+      <c r="C30" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="84"/>
+      <c r="D30" s="83"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="24"/>
-      <c r="H30" s="44"/>
+      <c r="H30" s="43"/>
     </row>
     <row r="31" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="79" t="s">
+      <c r="A31" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="79"/>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="39"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H31" s="40"/>
+      <c r="H31" s="39"/>
     </row>
     <row r="32" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
@@ -3932,25 +3940,25 @@
       <c r="C32" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="40"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="39"/>
     </row>
     <row r="33" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="59" t="s">
+      <c r="C33" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="59"/>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83"/>
-      <c r="G33" s="83"/>
-      <c r="H33" s="43"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="42"/>
     </row>
     <row r="34" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -3960,21 +3968,21 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="43"/>
+      <c r="H34" s="42"/>
     </row>
     <row r="35" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="80" t="s">
+      <c r="A35" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="80"/>
-      <c r="C35" s="80"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="38"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="37"/>
       <c r="G35" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H35" s="45"/>
+      <c r="H35" s="44"/>
     </row>
     <row r="36" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
@@ -3984,25 +3992,25 @@
       <c r="C36" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="88"/>
       <c r="G36" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H36" s="45"/>
+      <c r="H36" s="44"/>
     </row>
     <row r="37" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="18"/>
       <c r="C37" s="17"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
+      <c r="D37" s="88"/>
+      <c r="E37" s="88"/>
+      <c r="F37" s="88"/>
       <c r="G37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H37" s="45"/>
+      <c r="H37" s="44"/>
     </row>
     <row r="38" spans="1:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
@@ -4012,68 +4020,68 @@
       <c r="E38" s="20"/>
       <c r="F38" s="20"/>
       <c r="G38" s="20"/>
-      <c r="H38" s="46"/>
+      <c r="H38" s="45"/>
     </row>
     <row r="39" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="77" t="s">
+      <c r="A39" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="77"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="85"/>
+      <c r="E39" s="85"/>
+      <c r="F39" s="85"/>
       <c r="G39" s="21"/>
-      <c r="H39" s="46"/>
+      <c r="H39" s="45"/>
     </row>
     <row r="40" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="22"/>
-      <c r="C40" s="83"/>
-      <c r="D40" s="83"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="83"/>
-      <c r="H40" s="41"/>
+      <c r="C40" s="80"/>
+      <c r="D40" s="80"/>
+      <c r="E40" s="80"/>
+      <c r="F40" s="80"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="40"/>
     </row>
     <row r="41" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
       <c r="B41" s="22"/>
-      <c r="C41" s="83"/>
-      <c r="D41" s="83"/>
-      <c r="E41" s="83"/>
-      <c r="F41" s="83"/>
-      <c r="G41" s="83"/>
-      <c r="H41" s="41"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="80"/>
+      <c r="E41" s="80"/>
+      <c r="F41" s="80"/>
+      <c r="G41" s="80"/>
+      <c r="H41" s="40"/>
     </row>
     <row r="42" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="84" t="s">
+      <c r="A43" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="84"/>
-      <c r="C43" s="84" t="s">
+      <c r="B43" s="83"/>
+      <c r="C43" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="84"/>
+      <c r="D43" s="83"/>
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
       <c r="G43" s="24"/>
-      <c r="H43" s="44"/>
+      <c r="H43" s="43"/>
     </row>
     <row r="44" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="79" t="s">
+      <c r="A44" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="79"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="79"/>
-      <c r="E44" s="79"/>
-      <c r="F44" s="39"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="87"/>
+      <c r="D44" s="87"/>
+      <c r="E44" s="87"/>
+      <c r="F44" s="38"/>
       <c r="G44" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H44" s="40"/>
+      <c r="H44" s="39"/>
     </row>
     <row r="45" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
@@ -4083,25 +4091,25 @@
       <c r="C45" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="83"/>
-      <c r="E45" s="83"/>
-      <c r="F45" s="83"/>
-      <c r="G45" s="83"/>
-      <c r="H45" s="40"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="80"/>
+      <c r="H45" s="39"/>
     </row>
     <row r="46" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="59" t="s">
+      <c r="C46" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D46" s="59"/>
-      <c r="E46" s="83"/>
-      <c r="F46" s="83"/>
-      <c r="G46" s="83"/>
-      <c r="H46" s="43"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="80"/>
+      <c r="F46" s="80"/>
+      <c r="G46" s="80"/>
+      <c r="H46" s="42"/>
     </row>
     <row r="47" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
@@ -4111,21 +4119,21 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="43"/>
+      <c r="H47" s="42"/>
     </row>
     <row r="48" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="80" t="s">
+      <c r="A48" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="80"/>
-      <c r="C48" s="80"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="38"/>
+      <c r="B48" s="86"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="86"/>
+      <c r="E48" s="86"/>
+      <c r="F48" s="37"/>
       <c r="G48" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H48" s="45"/>
+      <c r="H48" s="44"/>
     </row>
     <row r="49" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
@@ -4135,25 +4143,25 @@
       <c r="C49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D49" s="81"/>
-      <c r="E49" s="81"/>
-      <c r="F49" s="81"/>
+      <c r="D49" s="88"/>
+      <c r="E49" s="88"/>
+      <c r="F49" s="88"/>
       <c r="G49" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H49" s="45"/>
+      <c r="H49" s="44"/>
     </row>
     <row r="50" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="18"/>
       <c r="C50" s="17"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="81"/>
+      <c r="D50" s="88"/>
+      <c r="E50" s="88"/>
+      <c r="F50" s="88"/>
       <c r="G50" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H50" s="45"/>
+      <c r="H50" s="44"/>
     </row>
     <row r="51" spans="1:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="19"/>
@@ -4163,56 +4171,56 @@
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
-      <c r="H51" s="46"/>
+      <c r="H51" s="45"/>
     </row>
     <row r="52" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="77" t="s">
+      <c r="A52" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="B52" s="77"/>
-      <c r="C52" s="77"/>
-      <c r="D52" s="78"/>
-      <c r="E52" s="78"/>
-      <c r="F52" s="78"/>
+      <c r="B52" s="84"/>
+      <c r="C52" s="84"/>
+      <c r="D52" s="85"/>
+      <c r="E52" s="85"/>
+      <c r="F52" s="85"/>
       <c r="G52" s="21"/>
-      <c r="H52" s="46"/>
+      <c r="H52" s="45"/>
     </row>
     <row r="53" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="49"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="86"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="87"/>
-      <c r="F53" s="87"/>
-      <c r="G53" s="87"/>
-      <c r="H53" s="50"/>
+      <c r="A53" s="48"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="78"/>
+      <c r="D53" s="78"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="79"/>
+      <c r="H53" s="49"/>
     </row>
     <row r="54" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22"/>
       <c r="B54" s="22"/>
-      <c r="C54" s="83"/>
-      <c r="D54" s="83"/>
-      <c r="E54" s="83"/>
-      <c r="F54" s="83"/>
-      <c r="G54" s="83"/>
-      <c r="H54" s="41"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="80"/>
+      <c r="G54" s="80"/>
+      <c r="H54" s="40"/>
     </row>
     <row r="55" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="88"/>
-      <c r="D55" s="88"/>
+      <c r="C55" s="81"/>
+      <c r="D55" s="81"/>
     </row>
     <row r="56" spans="1:8" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27"/>
       <c r="B56" s="27"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
       <c r="E56" s="27"/>
       <c r="F56" s="27"/>
       <c r="G56" s="27"/>
-      <c r="H56" s="42"/>
+      <c r="H56" s="41"/>
     </row>
     <row r="57" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20"/>
@@ -4222,36 +4230,36 @@
       <c r="E57" s="20"/>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
-      <c r="H57" s="46"/>
+      <c r="H57" s="45"/>
     </row>
     <row r="58" spans="1:8" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="84" t="s">
+      <c r="A59" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="B59" s="84"/>
-      <c r="C59" s="84" t="s">
+      <c r="B59" s="83"/>
+      <c r="C59" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="D59" s="84"/>
+      <c r="D59" s="83"/>
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
       <c r="G59" s="24"/>
-      <c r="H59" s="44"/>
+      <c r="H59" s="43"/>
     </row>
     <row r="60" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="79" t="s">
+      <c r="A60" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B60" s="79"/>
-      <c r="C60" s="79"/>
-      <c r="D60" s="79"/>
-      <c r="E60" s="79"/>
-      <c r="F60" s="39"/>
+      <c r="B60" s="87"/>
+      <c r="C60" s="87"/>
+      <c r="D60" s="87"/>
+      <c r="E60" s="87"/>
+      <c r="F60" s="38"/>
       <c r="G60" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H60" s="40"/>
+      <c r="H60" s="39"/>
     </row>
     <row r="61" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
@@ -4261,25 +4269,25 @@
       <c r="C61" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D61" s="85"/>
-      <c r="E61" s="85"/>
-      <c r="F61" s="85"/>
-      <c r="G61" s="85"/>
-      <c r="H61" s="53"/>
+      <c r="D61" s="89"/>
+      <c r="E61" s="89"/>
+      <c r="F61" s="89"/>
+      <c r="G61" s="89"/>
+      <c r="H61" s="52"/>
     </row>
     <row r="62" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="59" t="s">
+      <c r="C62" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="59"/>
-      <c r="E62" s="83"/>
-      <c r="F62" s="83"/>
-      <c r="G62" s="83"/>
-      <c r="H62" s="43"/>
+      <c r="D62" s="71"/>
+      <c r="E62" s="80"/>
+      <c r="F62" s="80"/>
+      <c r="G62" s="80"/>
+      <c r="H62" s="42"/>
     </row>
     <row r="63" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
@@ -4289,21 +4297,21 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="43"/>
+      <c r="H63" s="42"/>
     </row>
     <row r="64" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="80" t="s">
+      <c r="A64" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="B64" s="80"/>
-      <c r="C64" s="80"/>
-      <c r="D64" s="80"/>
-      <c r="E64" s="80"/>
-      <c r="F64" s="38"/>
+      <c r="B64" s="86"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="86"/>
+      <c r="E64" s="86"/>
+      <c r="F64" s="37"/>
       <c r="G64" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H64" s="45"/>
+      <c r="H64" s="44"/>
     </row>
     <row r="65" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
@@ -4313,25 +4321,25 @@
       <c r="C65" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="83"/>
-      <c r="E65" s="83"/>
-      <c r="F65" s="83"/>
+      <c r="D65" s="80"/>
+      <c r="E65" s="80"/>
+      <c r="F65" s="80"/>
       <c r="G65" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H65" s="45"/>
+      <c r="H65" s="44"/>
     </row>
     <row r="66" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="18"/>
       <c r="C66" s="17"/>
-      <c r="D66" s="83"/>
-      <c r="E66" s="83"/>
-      <c r="F66" s="83"/>
+      <c r="D66" s="80"/>
+      <c r="E66" s="80"/>
+      <c r="F66" s="80"/>
       <c r="G66" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H66" s="45"/>
+      <c r="H66" s="44"/>
     </row>
     <row r="67" spans="1:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="19"/>
@@ -4341,47 +4349,92 @@
       <c r="E67" s="20"/>
       <c r="F67" s="20"/>
       <c r="G67" s="20"/>
-      <c r="H67" s="46"/>
+      <c r="H67" s="45"/>
     </row>
     <row r="68" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="77" t="s">
+      <c r="A68" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="B68" s="77"/>
-      <c r="C68" s="77"/>
-      <c r="D68" s="78"/>
-      <c r="E68" s="78"/>
-      <c r="F68" s="78"/>
+      <c r="B68" s="84"/>
+      <c r="C68" s="84"/>
+      <c r="D68" s="85"/>
+      <c r="E68" s="85"/>
+      <c r="F68" s="85"/>
       <c r="G68" s="21"/>
-      <c r="H68" s="46"/>
+      <c r="H68" s="45"/>
     </row>
     <row r="69" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="22"/>
       <c r="B69" s="22"/>
-      <c r="C69" s="83"/>
-      <c r="D69" s="83"/>
-      <c r="E69" s="83"/>
-      <c r="F69" s="83"/>
-      <c r="G69" s="83"/>
-      <c r="H69" s="41"/>
+      <c r="C69" s="80"/>
+      <c r="D69" s="80"/>
+      <c r="E69" s="80"/>
+      <c r="F69" s="80"/>
+      <c r="G69" s="80"/>
+      <c r="H69" s="40"/>
     </row>
     <row r="70" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="22"/>
       <c r="B70" s="22"/>
-      <c r="C70" s="83"/>
-      <c r="D70" s="83"/>
-      <c r="E70" s="83"/>
-      <c r="F70" s="83"/>
-      <c r="G70" s="83"/>
-      <c r="H70" s="41"/>
+      <c r="C70" s="80"/>
+      <c r="D70" s="80"/>
+      <c r="E70" s="80"/>
+      <c r="F70" s="80"/>
+      <c r="G70" s="80"/>
+      <c r="H70" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="D36:F37"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="D65:F66"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="D49:F50"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="D23:F24"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="A22:E22"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="A4:B4"/>
@@ -4393,56 +4446,11 @@
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="D10:F11"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="D23:F24"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="D49:F50"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="A60:E60"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="D65:F66"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="D36:F37"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.57291666666666663" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4455,10 +4463,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4498,240 +4506,293 @@
       <c r="A5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="90"/>
-    </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="97"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="54"/>
+      <c r="B6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="C6" s="29"/>
+      <c r="D6" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="29"/>
+    </row>
+    <row r="7" spans="1:9" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="55"/>
+      <c r="B7" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="32" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="29"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="91"/>
-      <c r="B7" s="93" t="s">
+      <c r="E7" s="30"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="90"/>
+      <c r="B8" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="95" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="92"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="31"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="24"/>
+      <c r="E8" s="30"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="91"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="90"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="B13" s="96"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="97"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="54"/>
+      <c r="B14" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="C14" s="29"/>
+      <c r="D14" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="55"/>
+      <c r="B15" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="32" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="29"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="91"/>
-      <c r="B15" s="93" t="s">
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="90"/>
+      <c r="B16" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="95" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="30"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="92"/>
-      <c r="B16" s="94"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="31"/>
+      <c r="E16" s="30"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="91"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="31"/>
+    </row>
+    <row r="18" spans="1:5" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="56"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="89"/>
-      <c r="C21" s="89"/>
-      <c r="D21" s="89"/>
-      <c r="E21" s="90"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
+      <c r="B21" s="96"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="97"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="54"/>
+      <c r="B22" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="C22" s="29"/>
+      <c r="D22" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="29"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="55"/>
+      <c r="B23" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="32" t="s">
+      <c r="C23" s="30"/>
+      <c r="D23" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="29"/>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="91"/>
-      <c r="B23" s="93" t="s">
+      <c r="E23" s="30"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="90"/>
+      <c r="B24" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="95" t="s">
+      <c r="C24" s="30"/>
+      <c r="D24" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="30"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="92"/>
-      <c r="B24" s="94"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="96"/>
-      <c r="E24" s="31"/>
+      <c r="E24" s="30"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="91"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="31"/>
+    </row>
+    <row r="26" spans="1:5" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="56"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="24"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="89"/>
-      <c r="C29" s="89"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="90"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="s">
+      <c r="B29" s="96"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="97"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="54"/>
+      <c r="B30" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="C30" s="29"/>
+      <c r="D30" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="29"/>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="55"/>
+      <c r="B31" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="32" t="s">
+      <c r="C31" s="30"/>
+      <c r="D31" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="29"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="91"/>
-      <c r="B31" s="93" t="s">
+      <c r="E31" s="30"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="90"/>
+      <c r="B32" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="95" t="s">
+      <c r="C32" s="30"/>
+      <c r="D32" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="30"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="92"/>
-      <c r="B32" s="94"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="96"/>
-      <c r="E32" s="31"/>
-    </row>
+      <c r="E32" s="30"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="91"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="31"/>
+    </row>
+    <row r="35" spans="1:5" s="51" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="89"/>
-      <c r="C37" s="89"/>
-      <c r="D37" s="89"/>
-      <c r="E37" s="90"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="55" t="s">
+      <c r="B37" s="96"/>
+      <c r="C37" s="96"/>
+      <c r="D37" s="96"/>
+      <c r="E37" s="97"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="54"/>
+      <c r="B38" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="C38" s="29"/>
+      <c r="D38" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="29"/>
+    </row>
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="55"/>
+      <c r="B39" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="32" t="s">
+      <c r="C39" s="30"/>
+      <c r="D39" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="29"/>
-    </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="91"/>
-      <c r="B39" s="93" t="s">
+      <c r="E39" s="30"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="90"/>
+      <c r="B40" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="95" t="s">
+      <c r="C40" s="30"/>
+      <c r="D40" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="E39" s="30"/>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="92"/>
-      <c r="B40" s="94"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="96"/>
-      <c r="E40" s="31"/>
+      <c r="E40" s="30"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="91"/>
+      <c r="B41" s="93"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="95"/>
+      <c r="E41" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>